<commit_message>
Se agrega proyecto para reclutamiento en hircasa
</commit_message>
<xml_diff>
--- a/datosClientes.xlsx
+++ b/datosClientes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hircasa-my.sharepoint.com/personal/agarcia_hircasa_com/Documents/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajcontrerasc\source\repos\HirCasaDesarrollo\Reclutamiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{D9E0C80F-6A70-415C-ADF8-BA4F005A81EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85091A71-CB42-4EEF-B20B-938F6E592A6B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61C7822-2FD7-4D3B-8EA6-17CAF7147FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30795" yWindow="11010" windowWidth="25860" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
   <si>
     <t>477-1943</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>Aprobación</t>
+  </si>
+  <si>
+    <t>pagosCliente 8</t>
   </si>
 </sst>
 </file>
@@ -827,31 +830,32 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1209,25 +1213,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1256,7 +1260,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1272,7 +1276,7 @@
       <c r="E2" s="3">
         <v>24</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>74300.039999999994</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1285,7 +1289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1301,7 +1305,7 @@
       <c r="E3" s="3">
         <v>18</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>1213748.2</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1314,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1330,7 +1334,7 @@
       <c r="E4" s="3">
         <v>45</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>378121.58</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1343,7 +1347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1359,7 +1363,7 @@
       <c r="E5" s="3">
         <v>39</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>22430.14</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -1372,7 +1376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1385,10 +1389,10 @@
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="3">
         <v>28</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>664419.39</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -1401,7 +1405,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1417,7 +1421,7 @@
       <c r="E7" s="3">
         <v>25</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>980000.5</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -1430,7 +1434,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1446,7 +1450,7 @@
       <c r="E8" s="3">
         <v>56</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>276899.83</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -1459,7 +1463,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1475,7 +1479,7 @@
       <c r="E9" s="3">
         <v>83</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>778564</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -1488,7 +1492,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1504,7 +1508,7 @@
       <c r="E10" s="3">
         <v>60</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>331876</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -1517,7 +1521,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1533,7 +1537,7 @@
       <c r="E11" s="3">
         <v>37</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>634567.19999999995</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -1546,274 +1550,274 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F101" s="1"/>
     </row>
   </sheetData>
@@ -1826,287 +1830,299 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
         <v>8</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="10">
         <v>898960.61</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="10">
         <v>10</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="10">
         <v>498882.82</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="10">
         <v>631239.4</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="G4" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="6">
+        <f>SUM(C2,C14)</f>
+        <v>912738.32</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10">
         <v>43000</v>
       </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="H5" s="10">
+        <v>778564</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="10">
         <v>5</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="10">
         <v>88656.6</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="10">
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="H6" s="6">
+        <f>H4-H5</f>
+        <v>134174.31999999995</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="10">
         <v>6</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="10">
         <v>254661.68</v>
       </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="10">
         <v>2</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="10">
         <v>50846.04</v>
       </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+      <c r="F8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="10">
         <v>7</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="10">
         <v>67764.009999999995</v>
       </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="10">
         <v>6</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="10">
         <v>669890.81999999995</v>
       </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+      <c r="F10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10">
         <v>2700</v>
       </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="10">
         <v>9</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="10">
         <v>331876</v>
       </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="10">
         <v>8</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="10">
         <v>787879.68</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="10">
         <v>0</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>8</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="6">
         <v>13777.71</v>
       </c>
       <c r="D14" s="3">
@@ -2115,17 +2131,17 @@
       <c r="E14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3">
         <v>4</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="6">
         <v>8372.77</v>
       </c>
       <c r="D15" s="3">
@@ -2135,14 +2151,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="6">
         <v>7298</v>
       </c>
       <c r="D16" s="3">
@@ -2152,14 +2168,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3">
         <v>4</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="6">
         <v>2572.31</v>
       </c>
       <c r="D17" s="3">
@@ -2169,14 +2185,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3">
         <v>10</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="6">
         <v>447671.39</v>
       </c>
       <c r="D18" s="3">
@@ -2185,16 +2201,16 @@
       <c r="E18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3">
         <v>6</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="6">
         <v>197670.39999999999</v>
       </c>
       <c r="D19" s="3">
@@ -2204,14 +2220,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="3">
         <v>10</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="6">
         <v>490376.34</v>
       </c>
       <c r="D20" s="3">
@@ -2221,14 +2237,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="6">
         <v>326830.23</v>
       </c>
       <c r="D21" s="3">
@@ -2237,16 +2253,16 @@
       <c r="E21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="6">
         <v>1713.89</v>
       </c>
       <c r="D22" s="3">
@@ -2256,14 +2272,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="6">
         <v>1000.04</v>
       </c>
       <c r="D23" s="3">
@@ -2273,14 +2289,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="3">
         <v>3</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="6">
         <v>66661.37</v>
       </c>
       <c r="D24" s="3">
@@ -2289,16 +2305,16 @@
       <c r="E24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="3">
         <v>2</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="6">
         <v>238787.18</v>
       </c>
       <c r="D25" s="3">
@@ -2308,14 +2324,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="3">
         <v>5</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="6">
         <v>255220.05</v>
       </c>
       <c r="D26" s="3">
@@ -2325,14 +2341,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="3">
         <v>3</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="6">
         <v>68767.62</v>
       </c>
       <c r="D27" s="3">
@@ -2341,16 +2357,16 @@
       <c r="E27" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="3">
         <v>7</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="6">
         <v>137308.5</v>
       </c>
       <c r="D28" s="3">
@@ -2360,14 +2376,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="6">
         <v>20000</v>
       </c>
       <c r="D29" s="3">
@@ -2376,16 +2392,16 @@
       <c r="E29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="3">
         <v>2</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>14578.38</v>
       </c>
       <c r="D30" s="3">
@@ -2395,14 +2411,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="3">
         <v>6</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="6">
         <v>64488.01</v>
       </c>
       <c r="D31" s="3">
@@ -2411,146 +2427,144 @@
       <c r="E31" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="10">
         <v>4</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="10">
         <v>8264.7199999999993</v>
       </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="D32" s="10">
+        <v>1</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3">
+    <row r="33" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="10">
         <v>3</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="10">
         <v>348887.74</v>
       </c>
-      <c r="D33" s="3">
-        <v>1</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="D33" s="10">
+        <v>1</v>
+      </c>
+      <c r="E33" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
+    <row r="34" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="10">
         <v>2</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="10">
         <v>555687.92000000004</v>
       </c>
-      <c r="D34" s="3">
-        <v>1</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="D34" s="10">
+        <v>1</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3">
+    </row>
+    <row r="35" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
         <v>34</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="10">
         <v>6</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="10">
         <v>537766.31999999995</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="10">
         <v>0</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3">
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
         <v>35</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="10">
         <v>10</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="10">
         <v>327769.86</v>
       </c>
-      <c r="D36" s="3">
-        <v>1</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3">
+    <row r="37" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
         <v>36</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="10">
         <v>2</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="10">
         <v>31543.759999999998</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="10">
         <v>0</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="3">
+    <row r="38" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
         <v>37</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="10">
         <v>2</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="10">
         <v>255678.57</v>
       </c>
-      <c r="D38" s="3">
-        <v>1</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="3">
+    <row r="39" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
         <v>38</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="10">
         <v>5</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="10">
         <v>366888.15</v>
       </c>
-      <c r="D39" s="3">
-        <v>1</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D39" s="10">
+        <v>1</v>
+      </c>
+      <c r="E39" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F39" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E39" xr:uid="{00000000-0009-0000-0000-000001000000}">
@@ -2576,165 +2590,165 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>8</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>912738</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>-134174</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>5</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>